<commit_message>
-ref TypeRepository::GetTypeWithMap -tests success
</commit_message>
<xml_diff>
--- a/Tests/WorkSpeed.Tests/WarehouseTests/TestFiles/products.xlsx
+++ b/Tests/WorkSpeed.Tests/WarehouseTests/TestFiles/products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WorkSpeed\Tests\WorkSpeed.Tests\WarehouseTests\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8619E92-EAD8-4FF3-BB3F-84D3AE02B736}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96F0246-A0AC-4A80-A766-9B423ADCD568}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,12 +499,20 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="101" customWidth="1"/>
+    <col min="3" max="3" width="61" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
     <col min="18" max="18" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>